<commit_message>
Implement status update service     - Update to connection pool     - Add npm script for DB setup
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A81BA83-704A-4AD4-B4AA-C806C1DCF0BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{482DA957-001D-4389-AEE1-CB9F0280E044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>Longest Substring Without Repeating Characters</t>
   </si>
@@ -69,6 +69,105 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/regular-expression-matching</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/median-of-two-sorted-arrays</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/container-with-most-water</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum</t>
+  </si>
+  <si>
+    <t>3Sum Closest</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum-closest</t>
+  </si>
+  <si>
+    <t>4Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/4sum</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-array</t>
+  </si>
+  <si>
+    <t>Remove Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-element</t>
+  </si>
+  <si>
+    <t>Next Permutation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/next-permutation</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-insert-position</t>
+  </si>
+  <si>
+    <t>Height Checker</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/height-checker</t>
+  </si>
+  <si>
+    <t>counting-sort</t>
+  </si>
+  <si>
+    <t>Relative Sort Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/relative-sort-array</t>
+  </si>
+  <si>
+    <t>Plus One</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/plus-one</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/pascals-triangle-ii</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number</t>
   </si>
 </sst>
 </file>
@@ -420,13 +519,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="48.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -513,6 +618,261 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>